<commit_message>
Fixed all files, added LMG and polygon
</commit_message>
<xml_diff>
--- a/timings.xlsx
+++ b/timings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13635" activeTab="1"/>
+    <workbookView windowWidth="14265" windowHeight="13185" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="8-9" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161">
   <si>
     <t>MIKAN</t>
   </si>
@@ -230,6 +230,9 @@
     <t>KNEVA</t>
   </si>
   <si>
+    <t>19:50:00</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 21:50:00</t>
   </si>
   <si>
@@ -239,6 +242,15 @@
     <t xml:space="preserve"> 20:10:00</t>
   </si>
   <si>
+    <t>21:10:00</t>
+  </si>
+  <si>
+    <t>20:00:00</t>
+  </si>
+  <si>
+    <t>01:20:00</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 01:50:00</t>
   </si>
   <si>
@@ -254,48 +266,117 @@
     <t>STAIV</t>
   </si>
   <si>
+    <t>01:10:00</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 02:20:00</t>
   </si>
   <si>
     <t xml:space="preserve"> 20:30:00</t>
   </si>
   <si>
+    <t>20:40:00</t>
+  </si>
+  <si>
     <t>KNESA</t>
   </si>
   <si>
     <t>POPLA</t>
   </si>
   <si>
+    <t>22:30:00</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 00:00:00</t>
   </si>
   <si>
+    <t>00:15:00</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 21:40:00</t>
   </si>
   <si>
+    <t>19:25:00</t>
+  </si>
+  <si>
+    <t>21:30:00</t>
+  </si>
+  <si>
+    <t>19:40:00</t>
+  </si>
+  <si>
+    <t>23:50:00</t>
+  </si>
+  <si>
+    <t>00:30:00</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 22:20:00</t>
   </si>
   <si>
+    <t>22:50:00</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 02:30:00</t>
   </si>
   <si>
     <t>CIRNI</t>
   </si>
   <si>
+    <t>19:45:00</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 21:10:00</t>
   </si>
   <si>
+    <t>22:10:00</t>
+  </si>
+  <si>
+    <t>21:20:00</t>
+  </si>
+  <si>
+    <t>23:20:00</t>
+  </si>
+  <si>
+    <t>00:13:00</t>
+  </si>
+  <si>
+    <t>01:45:00</t>
+  </si>
+  <si>
+    <t>19:53:00</t>
+  </si>
+  <si>
+    <t>01:40:00</t>
+  </si>
+  <si>
+    <t>19:44:00</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 21:30:00</t>
   </si>
   <si>
+    <t>01:30:00</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 00:10:00</t>
   </si>
   <si>
+    <t>19:30:00</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 20:50:00</t>
   </si>
   <si>
+    <t>22:20:00</t>
+  </si>
+  <si>
     <t>TESAL</t>
   </si>
   <si>
+    <t>00:00:00</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 21:15:00</t>
   </si>
   <si>
@@ -356,16 +437,28 @@
     <t xml:space="preserve">22:36:00 </t>
   </si>
   <si>
+    <t>00:40:00</t>
+  </si>
+  <si>
     <t>MIRAL</t>
   </si>
   <si>
     <t>BASML</t>
   </si>
   <si>
+    <t>19:20:00</t>
+  </si>
+  <si>
+    <t>22:40:00</t>
+  </si>
+  <si>
     <t>VUKDU</t>
   </si>
   <si>
     <t xml:space="preserve"> 20:00:00</t>
+  </si>
+  <si>
+    <t>20:10:00</t>
   </si>
   <si>
     <t xml:space="preserve">22:47:00 </t>
@@ -419,9 +512,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -447,6 +540,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -458,13 +558,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -485,9 +578,62 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -502,38 +648,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -541,43 +671,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -598,13 +691,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -616,13 +727,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -640,7 +751,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -652,19 +781,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -676,13 +817,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -694,19 +829,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -718,55 +859,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -810,13 +903,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -824,8 +936,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -848,89 +960,70 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="27" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6"/>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5"/>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0"/>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3"/>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="7"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="8"/>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="5"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5"/>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3"/>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="6"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="6"/>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -952,7 +1045,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="35" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1016,10 +1109,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="2D2D2D"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FCFCFC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1504,7 +1597,7 @@
   <sheetPr/>
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -1693,7 +1786,7 @@
   <dimension ref="A1:U32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -2113,11 +2206,11 @@
       <c r="A15" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="6">
-        <v>0.826388888888889</v>
+      <c r="B15" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -2140,10 +2233,10 @@
     </row>
     <row r="16" s="3" customFormat="1" spans="1:21">
       <c r="A16" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B16" s="6">
-        <v>0.826388888888889</v>
+        <v>71</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>50</v>
@@ -2171,11 +2264,11 @@
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="6">
-        <v>0.826388888888889</v>
+      <c r="B17" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -2200,8 +2293,8 @@
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="6">
-        <v>0.881944444444444</v>
+      <c r="B18" s="6" t="s">
+        <v>73</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>50</v>
@@ -2229,8 +2322,8 @@
       <c r="A19" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="6">
-        <v>0.833333333333333</v>
+      <c r="B19" s="6" t="s">
+        <v>74</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>50</v>
@@ -2258,11 +2351,11 @@
       <c r="A20" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="6">
-        <v>0.0555555555555556</v>
+      <c r="B20" s="6" t="s">
+        <v>75</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -2285,13 +2378,13 @@
     </row>
     <row r="21" s="3" customFormat="1" spans="1:21">
       <c r="A21" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B21" s="6">
-        <v>0.826388888888889</v>
+        <v>77</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -2316,11 +2409,11 @@
       <c r="A22" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="6">
-        <v>0.826388888888889</v>
+      <c r="B22" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -2345,11 +2438,11 @@
       <c r="A23" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="6">
-        <v>0.902777777777778</v>
+      <c r="B23" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -2374,8 +2467,8 @@
       <c r="A24" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="6">
-        <v>0.909722222222222</v>
+      <c r="B24" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>53</v>
@@ -2403,8 +2496,8 @@
       <c r="A25" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="6">
-        <v>0.826388888888889</v>
+      <c r="B25" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>50</v>
@@ -2430,13 +2523,13 @@
     </row>
     <row r="26" s="3" customFormat="1" spans="1:21">
       <c r="A26" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B26" s="6">
-        <v>0.0486111111111111</v>
+        <v>80</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -2461,8 +2554,8 @@
       <c r="A27" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="6">
-        <v>0.826388888888889</v>
+      <c r="B27" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>50</v>
@@ -2490,11 +2583,11 @@
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="6">
-        <v>0.826388888888889</v>
+      <c r="B28" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -2519,11 +2612,11 @@
       <c r="A29" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="6">
-        <v>0.861111111111111</v>
+      <c r="B29" s="6" t="s">
+        <v>84</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -2546,10 +2639,10 @@
     </row>
     <row r="30" s="3" customFormat="1" spans="1:21">
       <c r="A30" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B30" s="6">
-        <v>0.826388888888889</v>
+        <v>85</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>50</v>
@@ -2577,11 +2670,11 @@
       <c r="A31" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="6">
-        <v>0.826388888888889</v>
+      <c r="B31" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -2606,8 +2699,8 @@
       <c r="A32" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="6">
-        <v>0.826388888888889</v>
+      <c r="B32" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>50</v>
@@ -2642,8 +2735,8 @@
   <sheetPr/>
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="2"/>
@@ -2655,23 +2748,23 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B1" s="6">
-        <v>0.9375</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>81</v>
+        <v>86</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="6">
-        <v>0.0104166666666667</v>
-      </c>
-      <c r="C2" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2679,43 +2772,43 @@
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="6">
-        <v>0.833333333333333</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>82</v>
+      <c r="B3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="6">
-        <v>0.909722222222222</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B5" s="6">
-        <v>0.809027777777778</v>
-      </c>
-      <c r="C5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0.895833333333333</v>
-      </c>
-      <c r="C6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2723,10 +2816,10 @@
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="6">
-        <v>0.819444444444444</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2734,10 +2827,10 @@
       <c r="A8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="6">
-        <v>0.902777777777778</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="B8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2745,10 +2838,10 @@
       <c r="A9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="6">
-        <v>0.993055555555556</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="B9" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2756,21 +2849,21 @@
       <c r="A10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="6">
-        <v>0.0208333333333333</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="B10" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B11" s="6">
-        <v>0.809027777777778</v>
-      </c>
-      <c r="C11" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2778,43 +2871,43 @@
       <c r="A12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="6">
-        <v>0.826388888888889</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>83</v>
+      <c r="B12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="6">
-        <v>0.951388888888889</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>84</v>
+      <c r="B13" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B14" s="6">
-        <v>0.822916666666667</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>86</v>
+        <v>99</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B15" s="6">
-        <v>0.923611111111111</v>
-      </c>
-      <c r="C15" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2822,10 +2915,10 @@
       <c r="A16" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="6">
-        <v>0.888888888888889</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="B16" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2833,21 +2926,21 @@
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="6">
-        <v>0.972222222222222</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>81</v>
+      <c r="B17" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="6">
-        <v>0.00902777777777778</v>
-      </c>
-      <c r="C18" s="3" t="s">
+      <c r="B18" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2855,10 +2948,10 @@
       <c r="A19" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="6">
-        <v>0.0486111111111111</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="B19" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2866,21 +2959,21 @@
       <c r="A20" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="6">
-        <v>0.0729166666666667</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>77</v>
+      <c r="B20" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="6">
-        <v>0.828472222222222</v>
-      </c>
-      <c r="C21" s="3" t="s">
+      <c r="B21" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2888,10 +2981,10 @@
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="6">
-        <v>0.0138888888888889</v>
-      </c>
-      <c r="C22" s="3" t="s">
+      <c r="B22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2899,21 +2992,21 @@
       <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="6">
-        <v>0.0694444444444444</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>84</v>
+      <c r="B23" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="6">
-        <v>0.822916666666667</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="B24" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>53</v>
       </c>
     </row>
@@ -2921,21 +3014,21 @@
       <c r="A25" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="6">
-        <v>0.822222222222222</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>87</v>
+      <c r="B25" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="6">
-        <v>0.819444444444444</v>
-      </c>
-      <c r="C26" s="3" t="s">
+      <c r="B26" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2943,21 +3036,21 @@
       <c r="A27" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="6">
-        <v>0.909722222222222</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>75</v>
+      <c r="B27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="6">
-        <v>0.0625</v>
-      </c>
-      <c r="C28" s="3" t="s">
+      <c r="B28" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2965,10 +3058,10 @@
       <c r="A29" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="6">
-        <v>0.826388888888889</v>
-      </c>
-      <c r="C29" s="3" t="s">
+      <c r="B29" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2976,32 +3069,32 @@
       <c r="A30" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="6">
-        <v>0.9375</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>88</v>
+      <c r="B30" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="6">
-        <v>0.8125</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>89</v>
+      <c r="B31" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="6">
-        <v>0.909722222222222</v>
-      </c>
-      <c r="C32" s="3" t="s">
+      <c r="B32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>67</v>
       </c>
     </row>
@@ -3009,21 +3102,21 @@
       <c r="A33" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="6">
-        <v>0.930555555555556</v>
-      </c>
-      <c r="C33" s="3" t="s">
+      <c r="B33" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B34" s="6">
-        <v>0.923611111111111</v>
-      </c>
-      <c r="C34" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3031,10 +3124,10 @@
       <c r="A35" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B35" s="6">
-        <v>0.833333333333333</v>
-      </c>
-      <c r="C35" s="3" t="s">
+      <c r="B35" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>60</v>
       </c>
     </row>
@@ -3042,10 +3135,10 @@
       <c r="A36" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B36" s="6">
-        <v>0.888888888888889</v>
-      </c>
-      <c r="C36" s="3" t="s">
+      <c r="B36" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>50</v>
       </c>
     </row>
@@ -3053,10 +3146,10 @@
       <c r="A37" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="6">
-        <v>0.923611111111111</v>
-      </c>
-      <c r="C37" s="3" t="s">
+      <c r="B37" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3064,10 +3157,10 @@
       <c r="A38" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="6">
-        <v>0.0208333333333333</v>
-      </c>
-      <c r="C38" s="3" t="s">
+      <c r="B38" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -3075,43 +3168,43 @@
       <c r="A39" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B39" s="6">
-        <v>0.0694444444444444</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>84</v>
+      <c r="B39" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="6">
-        <v>0.826388888888889</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>86</v>
+      <c r="B40" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B41" s="6">
-        <v>0.819444444444444</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>75</v>
+      <c r="B41" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B42" s="6">
-        <v>0</v>
-      </c>
-      <c r="C42" s="3" t="s">
+      <c r="B42" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3119,21 +3212,21 @@
       <c r="A43" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B43" s="6">
-        <v>0.819444444444444</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>91</v>
+      <c r="B43" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B44" s="6">
-        <v>0.951388888888889</v>
-      </c>
-      <c r="C44" s="3" t="s">
+      <c r="B44" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3141,32 +3234,32 @@
       <c r="A45" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B45" s="6">
-        <v>0.819444444444444</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>75</v>
+      <c r="B45" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B46" s="6">
-        <v>0</v>
-      </c>
-      <c r="C46" s="3" t="s">
+      <c r="B46" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B47" s="6">
-        <v>0.819444444444444</v>
-      </c>
-      <c r="C47" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3182,7 +3275,7 @@
   <dimension ref="A1:U48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -3198,7 +3291,7 @@
         <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>50</v>
@@ -3227,10 +3320,10 @@
         <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>93</v>
+        <v>120</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>94</v>
+        <v>121</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -3259,7 +3352,7 @@
         <v>49</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -3282,13 +3375,13 @@
     </row>
     <row r="4" s="3" customFormat="1" spans="1:21">
       <c r="A4" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>95</v>
+        <v>122</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -3311,7 +3404,7 @@
     </row>
     <row r="5" s="3" customFormat="1" spans="1:21">
       <c r="A5" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>34</v>
@@ -3340,13 +3433,13 @@
     </row>
     <row r="6" s="3" customFormat="1" spans="1:21">
       <c r="A6" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -3369,13 +3462,13 @@
     </row>
     <row r="7" s="3" customFormat="1" spans="1:21">
       <c r="A7" s="1" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>63</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -3398,10 +3491,10 @@
     </row>
     <row r="8" s="3" customFormat="1" spans="1:21">
       <c r="A8" s="1" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>53</v>
@@ -3427,7 +3520,7 @@
     </row>
     <row r="9" s="3" customFormat="1" spans="1:21">
       <c r="A9" s="1" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>6</v>
@@ -3456,13 +3549,13 @@
     </row>
     <row r="10" s="3" customFormat="1" spans="1:21">
       <c r="A10" s="1" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -3485,10 +3578,10 @@
     </row>
     <row r="11" s="3" customFormat="1" spans="1:21">
       <c r="A11" s="1" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>98</v>
+        <v>125</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>45</v>
@@ -3514,10 +3607,10 @@
     </row>
     <row r="12" s="3" customFormat="1" spans="1:21">
       <c r="A12" s="1" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>60</v>
@@ -3543,13 +3636,13 @@
     </row>
     <row r="13" s="3" customFormat="1" spans="1:21">
       <c r="A13" s="1" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>101</v>
+        <v>128</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>102</v>
+        <v>129</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -3572,13 +3665,13 @@
     </row>
     <row r="14" s="3" customFormat="1" spans="1:21">
       <c r="A14" s="1" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>103</v>
+        <v>130</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -3604,7 +3697,7 @@
         <v>32</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>95</v>
+        <v>122</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>48</v>
@@ -3662,10 +3755,10 @@
         <v>33</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -3691,7 +3784,7 @@
         <v>56</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>95</v>
+        <v>122</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>48</v>
@@ -3723,7 +3816,7 @@
         <v>63</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>87</v>
+        <v>110</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -3746,13 +3839,13 @@
     </row>
     <row r="20" s="3" customFormat="1" spans="1:21">
       <c r="A20" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>87</v>
+        <v>110</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -3775,10 +3868,10 @@
     </row>
     <row r="21" s="3" customFormat="1" spans="1:21">
       <c r="A21" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>105</v>
+        <v>132</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>41</v>
@@ -3810,7 +3903,7 @@
         <v>65</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -3836,10 +3929,10 @@
         <v>52</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -3865,7 +3958,7 @@
         <v>52</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>106</v>
+        <v>133</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>67</v>
@@ -3894,10 +3987,10 @@
         <v>52</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>108</v>
+        <v>135</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -3923,7 +4016,7 @@
         <v>21</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>109</v>
+        <v>136</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>50</v>
@@ -3952,10 +4045,10 @@
         <v>21</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>110</v>
+        <v>137</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>94</v>
+        <v>121</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -3978,13 +4071,13 @@
     </row>
     <row r="28" s="3" customFormat="1" spans="1:21">
       <c r="A28" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B28" s="6">
-        <v>0.833333333333333</v>
+        <v>80</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>87</v>
+        <v>110</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -4007,10 +4100,10 @@
     </row>
     <row r="29" s="3" customFormat="1" spans="1:21">
       <c r="A29" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B29" s="6">
-        <v>0.916666666666667</v>
+        <v>80</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>53</v>
@@ -4036,10 +4129,10 @@
     </row>
     <row r="30" s="3" customFormat="1" spans="1:21">
       <c r="A30" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B30" s="6">
-        <v>0.0277777777777778</v>
+        <v>80</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>138</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>11</v>
@@ -4065,10 +4158,10 @@
     </row>
     <row r="31" s="3" customFormat="1" spans="1:21">
       <c r="A31" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B31" s="6">
-        <v>0.0555555555555556</v>
+        <v>80</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>14</v>
@@ -4094,13 +4187,13 @@
     </row>
     <row r="32" s="3" customFormat="1" spans="1:21">
       <c r="A32" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B32" s="6">
-        <v>0.8125</v>
+        <v>139</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -4123,10 +4216,10 @@
     </row>
     <row r="33" s="3" customFormat="1" spans="1:21">
       <c r="A33" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B33" s="6">
-        <v>0.9375</v>
+        <v>139</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>53</v>
@@ -4152,10 +4245,10 @@
     </row>
     <row r="34" s="3" customFormat="1" spans="1:21">
       <c r="A34" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B34" s="6">
-        <v>0.8125</v>
+        <v>140</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>60</v>
@@ -4181,10 +4274,10 @@
     </row>
     <row r="35" s="3" customFormat="1" spans="1:21">
       <c r="A35" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B35" s="6">
-        <v>0.9375</v>
+        <v>140</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>53</v>
@@ -4212,11 +4305,11 @@
       <c r="A36" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B36" s="6">
-        <v>0.826388888888889</v>
+      <c r="B36" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -4241,11 +4334,11 @@
       <c r="A37" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="6">
-        <v>0.819444444444444</v>
+      <c r="B37" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -4270,11 +4363,11 @@
       <c r="A38" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B38" s="6">
-        <v>0.923611111111111</v>
+      <c r="B38" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -4299,11 +4392,11 @@
       <c r="A39" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B39" s="6">
-        <v>0.8125</v>
+      <c r="B39" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>87</v>
+        <v>110</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -4328,8 +4421,8 @@
       <c r="A40" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B40" s="6">
-        <v>0.923611111111111</v>
+      <c r="B40" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>67</v>
@@ -4357,8 +4450,8 @@
       <c r="A41" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B41" s="6">
-        <v>0.805555555555556</v>
+      <c r="B41" s="1" t="s">
+        <v>141</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>50</v>
@@ -4386,11 +4479,11 @@
       <c r="A42" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B42" s="6">
-        <v>0.944444444444444</v>
+      <c r="B42" s="1" t="s">
+        <v>142</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -4413,13 +4506,13 @@
     </row>
     <row r="43" s="3" customFormat="1" spans="1:21">
       <c r="A43" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B43" s="6">
-        <v>0.819444444444444</v>
+        <v>143</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>114</v>
+        <v>144</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -4442,10 +4535,10 @@
     </row>
     <row r="44" s="3" customFormat="1" spans="1:21">
       <c r="A44" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B44" s="6">
-        <v>0.840277777777778</v>
+        <v>143</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>48</v>
@@ -4471,13 +4564,13 @@
     </row>
     <row r="45" s="3" customFormat="1" spans="1:21">
       <c r="A45" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B45" s="6">
-        <v>0.951388888888889</v>
+        <v>143</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -4535,7 +4628,7 @@
         <v>24</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
@@ -4560,8 +4653,8 @@
       <c r="A48" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B48" s="6">
-        <v>0</v>
+      <c r="B48" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>16</v>
@@ -4597,7 +4690,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -4638,7 +4731,7 @@
     </row>
     <row r="2" s="3" customFormat="1" spans="1:21">
       <c r="A2" s="1" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>65</v>
@@ -4667,10 +4760,10 @@
     </row>
     <row r="3" s="3" customFormat="1" spans="1:21">
       <c r="A3" s="1" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>115</v>
+        <v>146</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>67</v>
@@ -4696,10 +4789,10 @@
     </row>
     <row r="4" s="3" customFormat="1" spans="1:21">
       <c r="A4" s="1" t="s">
-        <v>116</v>
+        <v>147</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
@@ -4728,7 +4821,7 @@
         <v>51</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>117</v>
+        <v>148</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>53</v>
@@ -4754,13 +4847,13 @@
     </row>
     <row r="6" s="3" customFormat="1" spans="1:21">
       <c r="A6" s="1" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>87</v>
+        <v>110</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -4783,7 +4876,7 @@
     </row>
     <row r="7" s="3" customFormat="1" spans="1:21">
       <c r="A7" s="1" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>61</v>
@@ -4844,10 +4937,10 @@
         <v>31</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -4870,10 +4963,10 @@
     </row>
     <row r="10" s="3" customFormat="1" spans="1:21">
       <c r="A10" s="1" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>50</v>
@@ -4899,7 +4992,7 @@
     </row>
     <row r="11" s="3" customFormat="1" spans="1:21">
       <c r="A11" s="1" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>24</v>
@@ -4928,13 +5021,13 @@
     </row>
     <row r="12" s="3" customFormat="1" spans="1:21">
       <c r="A12" s="1" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -4957,10 +5050,10 @@
     </row>
     <row r="13" s="3" customFormat="1" spans="1:21">
       <c r="A13" s="1" t="s">
-        <v>113</v>
+        <v>143</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>50</v>
@@ -4986,7 +5079,7 @@
     </row>
     <row r="14" s="3" customFormat="1" spans="1:21">
       <c r="A14" s="1" t="s">
-        <v>113</v>
+        <v>143</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>24</v>
@@ -5015,13 +5108,13 @@
     </row>
     <row r="15" s="3" customFormat="1" spans="1:21">
       <c r="A15" s="1" t="s">
-        <v>113</v>
+        <v>143</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -5044,10 +5137,10 @@
     </row>
     <row r="16" s="3" customFormat="1" spans="1:21">
       <c r="A16" s="1" t="s">
-        <v>112</v>
+        <v>140</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>50</v>
@@ -5073,10 +5166,10 @@
     </row>
     <row r="17" s="3" customFormat="1" spans="1:21">
       <c r="A17" s="1" t="s">
-        <v>112</v>
+        <v>140</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>93</v>
+        <v>120</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>66</v>
@@ -5105,10 +5198,10 @@
         <v>27</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>117</v>
+        <v>148</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -5137,7 +5230,7 @@
         <v>62</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>118</v>
+        <v>149</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -5160,13 +5253,13 @@
     </row>
     <row r="20" s="3" customFormat="1" spans="1:21">
       <c r="A20" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="C20" s="1" t="s">
-        <v>118</v>
+        <v>149</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -5192,10 +5285,10 @@
         <v>33</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>87</v>
+        <v>110</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -5221,10 +5314,10 @@
         <v>33</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>93</v>
+        <v>120</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>120</v>
+        <v>151</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -5250,10 +5343,10 @@
         <v>40</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -5286,7 +5379,7 @@
   <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -5301,10 +5394,10 @@
         <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>121</v>
+        <v>152</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -5330,10 +5423,10 @@
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -5356,13 +5449,13 @@
     </row>
     <row r="3" s="3" customFormat="1" spans="1:21">
       <c r="A3" s="1" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>122</v>
+        <v>153</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>123</v>
+        <v>154</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -5388,7 +5481,7 @@
         <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>124</v>
+        <v>155</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>48</v>
@@ -5475,7 +5568,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>117</v>
+        <v>148</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>60</v>
@@ -5504,10 +5597,10 @@
         <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>117</v>
+        <v>148</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -5533,10 +5626,10 @@
         <v>32</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>117</v>
+        <v>148</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -5562,10 +5655,10 @@
         <v>32</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>125</v>
+        <v>156</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>126</v>
+        <v>157</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -5588,13 +5681,13 @@
     </row>
     <row r="11" s="3" customFormat="1" spans="1:21">
       <c r="A11" s="1" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>117</v>
+        <v>148</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>87</v>
+        <v>110</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -5617,7 +5710,7 @@
     </row>
     <row r="12" s="3" customFormat="1" spans="1:21">
       <c r="A12" s="1" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>34</v>
@@ -5646,10 +5739,10 @@
     </row>
     <row r="13" s="3" customFormat="1" spans="1:21">
       <c r="A13" s="1" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>67</v>
@@ -5675,13 +5768,13 @@
     </row>
     <row r="14" s="3" customFormat="1" spans="1:21">
       <c r="A14" s="1" t="s">
-        <v>112</v>
+        <v>140</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -5704,7 +5797,7 @@
     </row>
     <row r="15" s="3" customFormat="1" spans="1:21">
       <c r="A15" s="1" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>34</v>
@@ -5733,13 +5826,13 @@
     </row>
     <row r="16" s="3" customFormat="1" spans="1:21">
       <c r="A16" s="1" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>127</v>
+        <v>158</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -5762,10 +5855,10 @@
     </row>
     <row r="17" s="3" customFormat="1" spans="1:21">
       <c r="A17" s="1" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>128</v>
+        <v>159</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>28</v>
@@ -5794,10 +5887,10 @@
         <v>31</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>122</v>
+        <v>153</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -5823,7 +5916,7 @@
         <v>51</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>117</v>
+        <v>148</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>53</v>
@@ -5855,7 +5948,7 @@
         <v>6</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>108</v>
+        <v>135</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -5881,10 +5974,10 @@
         <v>51</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>129</v>
+        <v>160</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -5910,7 +6003,7 @@
         <v>40</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>124</v>
+        <v>155</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>48</v>
@@ -6003,8 +6096,8 @@
   <sheetPr/>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelRow="2" outlineLevelCol="2"/>
@@ -6023,12 +6116,12 @@
         <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>112</v>
+        <v>140</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>62</v>
@@ -6045,7 +6138,7 @@
         <v>61</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>108</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>